<commit_message>
updated Test creation and email+rollnumber uniqness validation
</commit_message>
<xml_diff>
--- a/TestCases/TestConductandAssesment.xlsx
+++ b/TestCases/TestConductandAssesment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Management" sheetId="1" r:id="rId1"/>
@@ -217,12 +217,6 @@
   </si>
   <si>
     <t>To verify Name of the test and Proceed button.</t>
-  </si>
-  <si>
-    <t>Test name:123  or more than 150 characters or    an empty field</t>
-  </si>
-  <si>
-    <t>User should not be able to create test with invalid test data.</t>
   </si>
   <si>
     <t>TC_10_OnlineQuiz_generated_link</t>
@@ -669,142 +663,6 @@
     <t>To verify  Invalid email id.</t>
   </si>
   <si>
-    <t>1)Go to test page.                                                            2)Go to test registration page                  
-3)Enter email id  in email text field.                             4)Enter First Name                                                     5)Enter Last Name.                                             6)Enter Conact Number                                    7)Enter Gender.                                                          8)Enter country                                                     9)Enter Roll Number</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Email id: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">dipapromact.com(Not in format abc@siri.com),more than 255 characters,or an empty field)                                                                               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>First Name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> raj@guru(non-alphabetic charcters or more than 255 characters or an empty field)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Last Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:Shah*(non-alphabetic charcters or more than 255 characters or an empty field)                                                         </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DOB: year selected </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">current year or greater than current year 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Contact Number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:786354(&lt;&gt;10 digits  or coaints letters)          
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Roll Number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:@@@@@12 (invalid or an empty field)
-</t>
-    </r>
-  </si>
-  <si>
     <t>Student should not be able to register .error should be displayed.</t>
   </si>
   <si>
@@ -957,6 +815,12 @@
     <t>When Attendee clicks on End test button Test should be ended and and message should be displayed at end.</t>
   </si>
   <si>
+    <t>Test name:123  or more than 150 characters or    an empty field                                                     Already created Test name.</t>
+  </si>
+  <si>
+    <t>User should not be able to create test with existed name and invalid test data.</t>
+  </si>
+  <si>
     <r>
       <t>Test name:                                apptitude test@101                    Max-150 character</t>
     </r>
@@ -979,7 +843,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">   </t>
+      <t xml:space="preserve">                         </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Go to test page.                                                            2)Go to test registration page                  
+3)Enter email id  in email text field.                             4)Enter First Name                                                     5)Enter Last Name.                                             6)Enter Conact Number                                    7)Enter Gender.                                                          8)Enter country                                                     9)Enter Roll Number                                                          </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Email id: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">dipapromact.com(Not in format abc@siri.com),more than 255 characters,or an empty field)                                                                               </t>
     </r>
     <r>
       <rPr>
@@ -990,7 +881,127 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t/>
+      <t>First Name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> raj@guru(non-alphabetic charcters or more than 255 characters or an empty field)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:Shah*(non-alphabetic charcters or more than 255 characters or an empty field)                                                         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DOB: year selected </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">current year or greater than current year 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contact Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:786354(&lt;&gt;10 digits  or coaints letters)          
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Roll Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:@@@@@12 (invalid or an empty field)                                    #</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">same email and roll number combination as already existed.     
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -1535,6 +1546,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1543,6 +1560,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1592,27 +1618,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1627,6 +1632,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1968,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E21"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,14 +2016,14 @@
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="120"/>
-      <c r="E2" s="121" t="s">
+      <c r="D2" s="118"/>
+      <c r="E2" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="121" t="s">
+      <c r="F2" s="119" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="122" t="s">
@@ -2033,8 +2044,8 @@
         <v>6</v>
       </c>
       <c r="D3" s="126"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
       <c r="G3" s="122"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -2087,7 +2098,7 @@
       <c r="B6" s="132"/>
       <c r="C6" s="133"/>
       <c r="D6" s="133"/>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="120" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="130"/>
@@ -2103,7 +2114,7 @@
       <c r="B7" s="132"/>
       <c r="C7" s="133"/>
       <c r="D7" s="133"/>
-      <c r="E7" s="111"/>
+      <c r="E7" s="121"/>
       <c r="F7" s="131"/>
       <c r="G7" s="131"/>
       <c r="H7" s="13"/>
@@ -2179,10 +2190,10 @@
       </c>
     </row>
     <row r="11" spans="1:16384" s="37" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="113"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="35"/>
       <c r="D11" s="36"/>
       <c r="E11" s="35"/>
@@ -18576,7 +18587,7 @@
       <c r="C12" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="91" t="s">
+      <c r="D12" s="93" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="41" t="s">
@@ -18602,7 +18613,7 @@
       <c r="C13" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="92"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="41" t="s">
         <v>34</v>
       </c>
@@ -18628,7 +18639,7 @@
       <c r="C14" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="92"/>
+      <c r="D14" s="94"/>
       <c r="E14" s="41" t="s">
         <v>39</v>
       </c>
@@ -18652,7 +18663,7 @@
       <c r="C15" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="92"/>
+      <c r="D15" s="94"/>
       <c r="E15" s="41" t="s">
         <v>43</v>
       </c>
@@ -18676,7 +18687,7 @@
       <c r="C16" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="41" t="s">
         <v>47</v>
       </c>
@@ -18700,7 +18711,7 @@
       <c r="C17" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="94"/>
       <c r="E17" s="41" t="s">
         <v>51</v>
       </c>
@@ -18724,7 +18735,7 @@
       <c r="C18" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="93"/>
+      <c r="D18" s="95"/>
       <c r="E18" s="41" t="s">
         <v>55</v>
       </c>
@@ -18739,13 +18750,13 @@
       <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112" t="s">
+      <c r="A19" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="116"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="98"/>
       <c r="F19" s="45"/>
       <c r="G19" s="46"/>
       <c r="H19" s="47"/>
@@ -18755,7 +18766,7 @@
       <c r="L19" s="47"/>
       <c r="M19" s="48"/>
     </row>
-    <row r="20" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>8</v>
       </c>
@@ -18765,14 +18776,14 @@
       <c r="C20" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="117" t="s">
+      <c r="D20" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="118" t="s">
+      <c r="E20" s="116" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>61</v>
@@ -18783,7 +18794,7 @@
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
     </row>
-    <row r="21" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
         <v>9</v>
       </c>
@@ -18793,13 +18804,13 @@
       <c r="C21" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="94"/>
-      <c r="E21" s="119"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="117"/>
       <c r="F21" s="41" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="H21" s="52"/>
       <c r="I21" s="52"/>
@@ -18812,22 +18823,22 @@
         <v>10</v>
       </c>
       <c r="B22" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="E22" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="F22" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="54" t="s">
+      <c r="G22" s="41" t="s">
         <v>69</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>71</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="52"/>
@@ -18840,20 +18851,20 @@
         <v>11</v>
       </c>
       <c r="B23" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="41" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>74</v>
       </c>
       <c r="F23" s="55"/>
       <c r="G23" s="56" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H23" s="44"/>
       <c r="I23" s="44"/>
@@ -18866,18 +18877,18 @@
         <v>12</v>
       </c>
       <c r="B24" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="99"/>
+      <c r="E24" s="57" t="s">
         <v>76</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="94"/>
-      <c r="E24" s="57" t="s">
-        <v>78</v>
       </c>
       <c r="F24" s="56"/>
       <c r="G24" s="56" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
@@ -18890,16 +18901,16 @@
         <v>13</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" s="60"/>
       <c r="E25" s="61"/>
       <c r="F25" s="56"/>
       <c r="G25" s="56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H25" s="44"/>
       <c r="I25" s="44"/>
@@ -18908,13 +18919,13 @@
       <c r="L25" s="44"/>
     </row>
     <row r="26" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="95" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="96"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="99"/>
+      <c r="A26" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="101"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="104"/>
       <c r="F26" s="62"/>
       <c r="G26" s="63"/>
       <c r="H26" s="64"/>
@@ -18929,18 +18940,18 @@
         <v>14</v>
       </c>
       <c r="B27" s="67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F27" s="68"/>
       <c r="G27" s="69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="70" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -18948,28 +18959,28 @@
         <v>15</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" s="68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F28" s="68"/>
       <c r="G28" s="69" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="101"/>
-      <c r="C29" s="102"/>
-      <c r="D29" s="103"/>
-      <c r="E29" s="104"/>
+      <c r="A29" s="105" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="106"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="71"/>
       <c r="G29" s="72"/>
       <c r="H29" s="73"/>
@@ -18984,10 +18995,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>29</v>
@@ -18995,7 +19006,7 @@
       <c r="E30" s="75"/>
       <c r="F30" s="42"/>
       <c r="G30" s="43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
@@ -19004,13 +19015,13 @@
       <c r="L30" s="44"/>
     </row>
     <row r="31" spans="1:13" s="80" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="105" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="106"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="109"/>
+      <c r="A31" s="110" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="111"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="114"/>
       <c r="F31" s="76"/>
       <c r="G31" s="77"/>
       <c r="H31" s="78"/>
@@ -19025,22 +19036,22 @@
         <v>15</v>
       </c>
       <c r="B32" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="F32" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="81" t="s">
+      <c r="G32" s="43" t="s">
         <v>97</v>
-      </c>
-      <c r="F32" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="43" t="s">
-        <v>99</v>
       </c>
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
@@ -19053,20 +19064,20 @@
         <v>16</v>
       </c>
       <c r="B33" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="94"/>
+      <c r="E33" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="F33" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="92"/>
-      <c r="E33" s="81" t="s">
+      <c r="G33" s="43" t="s">
         <v>102</v>
-      </c>
-      <c r="F33" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="43" t="s">
-        <v>104</v>
       </c>
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
@@ -19079,18 +19090,18 @@
         <v>17</v>
       </c>
       <c r="B34" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="94"/>
+      <c r="E34" s="51" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="92"/>
-      <c r="E34" s="51" t="s">
-        <v>107</v>
       </c>
       <c r="F34" s="42"/>
       <c r="G34" s="43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
@@ -19103,18 +19114,18 @@
         <v>18</v>
       </c>
       <c r="B35" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="94"/>
+      <c r="E35" s="51" t="s">
         <v>109</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="92"/>
-      <c r="E35" s="51" t="s">
-        <v>111</v>
       </c>
       <c r="F35" s="42"/>
       <c r="G35" s="43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H35" s="44"/>
       <c r="I35" s="44"/>
@@ -19127,20 +19138,20 @@
         <v>19</v>
       </c>
       <c r="B36" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="95"/>
+      <c r="E36" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="F36" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="93"/>
-      <c r="E36" s="51" t="s">
+      <c r="G36" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="F36" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="G36" s="43" t="s">
-        <v>117</v>
       </c>
       <c r="H36" s="44"/>
       <c r="I36" s="44"/>
@@ -19153,17 +19164,17 @@
         <v>20</v>
       </c>
       <c r="B37" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="51" t="s">
         <v>118</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>120</v>
       </c>
       <c r="F37" s="42"/>
       <c r="G37" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
@@ -19176,17 +19187,17 @@
         <v>21</v>
       </c>
       <c r="B38" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="51" t="s">
         <v>122</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>124</v>
       </c>
       <c r="F38" s="42"/>
       <c r="G38" s="43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
@@ -19199,17 +19210,17 @@
         <v>22</v>
       </c>
       <c r="B39" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="51" t="s">
         <v>126</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="51" t="s">
-        <v>128</v>
       </c>
       <c r="F39" s="42"/>
       <c r="G39" s="43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H39" s="44"/>
       <c r="I39" s="44"/>
@@ -19222,17 +19233,17 @@
         <v>23</v>
       </c>
       <c r="B40" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="51" t="s">
         <v>130</v>
-      </c>
-      <c r="C40" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="51" t="s">
-        <v>132</v>
       </c>
       <c r="F40" s="42"/>
       <c r="G40" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H40" s="44"/>
       <c r="I40" s="44"/>
@@ -19242,19 +19253,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="F4:F7"/>
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:D8"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D12:D18"/>
     <mergeCell ref="A19:B19"/>
@@ -19267,6 +19276,8 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:E31"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D20:D21" location="'Question Management_Dashboard'!B27" display="refer here"/>
@@ -19288,8 +19299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19326,10 +19337,10 @@
       <c r="B2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="120"/>
+      <c r="D2" s="118"/>
       <c r="E2" s="122" t="s">
         <v>2</v>
       </c>
@@ -19351,7 +19362,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="125" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="126"/>
       <c r="E3" s="122"/>
@@ -19389,7 +19400,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="133" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D5" s="133"/>
       <c r="E5" s="17" t="s">
@@ -19408,7 +19419,7 @@
       <c r="B6" s="140"/>
       <c r="C6" s="133"/>
       <c r="D6" s="133"/>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="120" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="130"/>
@@ -19424,7 +19435,7 @@
       <c r="B7" s="140"/>
       <c r="C7" s="133"/>
       <c r="D7" s="133"/>
-      <c r="E7" s="111"/>
+      <c r="E7" s="121"/>
       <c r="F7" s="131"/>
       <c r="G7" s="131"/>
       <c r="H7" s="13"/>
@@ -19463,12 +19474,12 @@
     </row>
     <row r="10" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="136" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" s="137"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="116"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="98"/>
       <c r="F10" s="45"/>
       <c r="G10" s="46"/>
       <c r="H10" s="47"/>
@@ -19521,20 +19532,20 @@
         <v>1</v>
       </c>
       <c r="B12" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="115" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="E12" s="41" t="s">
         <v>138</v>
-      </c>
-      <c r="D12" s="117" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>140</v>
       </c>
       <c r="F12" s="90"/>
       <c r="G12" s="41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
@@ -19547,16 +19558,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D13" s="134"/>
       <c r="E13" s="41"/>
       <c r="F13" s="90"/>
       <c r="G13" s="41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H13" s="52"/>
       <c r="I13" s="52"/>
@@ -19566,12 +19577,12 @@
     </row>
     <row r="14" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="136" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B14" s="137"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="115"/>
-      <c r="E14" s="116"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="45"/>
       <c r="G14" s="46"/>
       <c r="H14" s="47"/>
@@ -19586,22 +19597,22 @@
         <v>5</v>
       </c>
       <c r="B15" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="E15" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="135" t="s">
+      <c r="F15" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="G15" s="41" t="s">
         <v>149</v>
-      </c>
-      <c r="F15" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>151</v>
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="52"/>
@@ -19609,25 +19620,25 @@
       <c r="K15" s="52"/>
       <c r="L15" s="52"/>
     </row>
-    <row r="16" spans="1:13" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="255" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <v>6</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D16" s="135"/>
       <c r="E16" s="41" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="F16" s="87" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="52"/>
@@ -19640,18 +19651,18 @@
         <v>7</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D17" s="135"/>
       <c r="E17" s="41" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H17" s="41"/>
       <c r="I17" s="52"/>
@@ -19661,12 +19672,12 @@
     </row>
     <row r="18" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="136" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B18" s="137"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="115"/>
-      <c r="E18" s="116"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="98"/>
       <c r="F18" s="45"/>
       <c r="G18" s="46"/>
       <c r="H18" s="47"/>
@@ -19681,20 +19692,20 @@
         <v>8</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="117" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="115" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F19" s="40"/>
       <c r="G19" s="41" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="52"/>
@@ -19707,18 +19718,18 @@
         <v>9</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="94"/>
+        <v>163</v>
+      </c>
+      <c r="D20" s="99"/>
       <c r="E20" s="41" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F20" s="40"/>
       <c r="G20" s="41" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H20" s="41"/>
       <c r="I20" s="52"/>
@@ -19731,16 +19742,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="94"/>
+        <v>167</v>
+      </c>
+      <c r="D21" s="99"/>
       <c r="E21" s="41"/>
       <c r="F21" s="40"/>
       <c r="G21" s="41" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="52"/>
@@ -19753,18 +19764,18 @@
         <v>11</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="D22" s="94"/>
+        <v>170</v>
+      </c>
+      <c r="D22" s="99"/>
       <c r="E22" s="41" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F22" s="40"/>
       <c r="G22" s="41" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="52"/>
@@ -19777,18 +19788,18 @@
         <v>12</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="D23" s="94"/>
+        <v>173</v>
+      </c>
+      <c r="D23" s="99"/>
       <c r="E23" s="41" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F23" s="40"/>
       <c r="G23" s="41" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H23" s="41"/>
       <c r="I23" s="52"/>
@@ -19801,18 +19812,18 @@
         <v>13</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="D24" s="94"/>
+        <v>176</v>
+      </c>
+      <c r="D24" s="99"/>
       <c r="E24" s="41" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="43" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
@@ -19826,16 +19837,16 @@
         <v>14</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D25" s="134"/>
       <c r="E25" s="41"/>
       <c r="F25" s="42"/>
       <c r="G25" s="43" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H25" s="44"/>
       <c r="I25" s="44"/>
@@ -19846,12 +19857,12 @@
     </row>
     <row r="26" spans="1:13" s="49" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="136" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B26" s="137"/>
-      <c r="C26" s="114"/>
-      <c r="D26" s="115"/>
-      <c r="E26" s="116"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="98"/>
       <c r="F26" s="45"/>
       <c r="G26" s="46"/>
       <c r="H26" s="47"/>
@@ -19866,20 +19877,20 @@
         <v>16</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="D27" s="117" t="s">
-        <v>68</v>
+        <v>184</v>
+      </c>
+      <c r="D27" s="115" t="s">
+        <v>66</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="43" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H27" s="44"/>
       <c r="I27" s="44"/>
@@ -19893,18 +19904,18 @@
         <v>17</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="D28" s="94"/>
+        <v>188</v>
+      </c>
+      <c r="D28" s="99"/>
       <c r="E28" s="41" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="43" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H28" s="44"/>
       <c r="I28" s="44"/>
@@ -19918,18 +19929,18 @@
         <v>18</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D29" s="134"/>
       <c r="E29" s="41" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="43" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H29" s="44"/>
       <c r="I29" s="44"/>

</xml_diff>